<commit_message>
Improve call queue audit
</commit_message>
<xml_diff>
--- a/frontend/public/call-queue-template.xlsx
+++ b/frontend/public/call-queue-template.xlsx
@@ -8,103 +8,6 @@
   <definedNames/>
   <calcPr/>
 </workbook>
-</file>
-
-<file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
-<comments xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <authors>
-    <author/>
-  </authors>
-  <commentList>
-    <comment authorId="0" ref="J1">
-      <text>
-        <t xml:space="preserve">Turn ON this option if you want callers to hear a recorded greeting before being connected to a group member.</t>
-      </text>
-    </comment>
-    <comment authorId="0" ref="K1">
-      <text>
-        <t xml:space="preserve">Incoming calls will hear the selected music whenever the connection takes more than a moment to complete.</t>
-      </text>
-    </comment>
-    <comment authorId="0" ref="L1">
-      <text>
-        <t xml:space="preserve">Turn on this option when you want callers to hear music whenever you put a call on hold.</t>
-      </text>
-    </comment>
-    <comment authorId="0" ref="M1">
-      <text>
-        <t xml:space="preserve">Interrupt audio periodically and play a message</t>
-      </text>
-    </comment>
-    <comment authorId="0" ref="N1">
-      <text>
-        <t xml:space="preserve">Message that plays when Interrupt Audio is turned ON.</t>
-      </text>
-    </comment>
-    <comment authorId="0" ref="O1">
-      <text>
-        <t xml:space="preserve">- Rotating: Regularly change the order that you ring available members to evenly distribute calls.
-- Simultaneous: Ring all available members at the same time. You can do this for up to 10 extensions.
-- Sequential: Ring available members one at a time in the order you set.</t>
-      </text>
-    </comment>
-    <comment authorId="0" ref="P1">
-      <text>
-        <t xml:space="preserve">If a member does not answer within this time period, the queue will move onto the next available member.</t>
-      </text>
-    </comment>
-    <comment authorId="0" ref="Q1">
-      <text>
-        <t xml:space="preserve">Maximum amount of time caller waits for an available member.</t>
-      </text>
-    </comment>
-    <comment authorId="0" ref="R1">
-      <text>
-        <t xml:space="preserve">This option specifies how long the system will wait after an agent completes a call before automatically setting their status to "Available" for a call. This gives the member time to make notes or otherwise follow up on a call.</t>
-      </text>
-    </comment>
-    <comment authorId="0" ref="S1">
-      <text>
-        <t xml:space="preserve">Allow members to change their availability for this specific queue.</t>
-      </text>
-    </comment>
-    <comment authorId="0" ref="T1">
-      <text>
-        <t xml:space="preserve">Maximum number of callers allowed before queue is full.</t>
-      </text>
-    </comment>
-    <comment authorId="0" ref="V1">
-      <text>
-        <t xml:space="preserve">Indicate which Extension or External Number should be routed to if you've selected either of those options for routing if the Queue is full.</t>
-      </text>
-    </comment>
-    <comment authorId="0" ref="W1">
-      <text>
-        <t xml:space="preserve">What to do with the call when the Total Ring Time is reached.</t>
-      </text>
-    </comment>
-    <comment authorId="0" ref="X1">
-      <text>
-        <t xml:space="preserve">Indicate which Extension or External Number should be routed to if you've selected either of those options for routing if the Max Time is reached.</t>
-      </text>
-    </comment>
-    <comment authorId="0" ref="Z1">
-      <text>
-        <t xml:space="preserve">Specify the users that will have access to the messages that this mailbox receives.</t>
-      </text>
-    </comment>
-    <comment authorId="0" ref="AB1">
-      <text>
-        <t xml:space="preserve">List who should receive an email notify them of a voicemail for the Queue. </t>
-      </text>
-    </comment>
-    <comment authorId="0" ref="AD1">
-      <text>
-        <t xml:space="preserve">Indicate which Extension or External Number should be routed to if you've selected either of those options for routing After Hours.</t>
-      </text>
-    </comment>
-  </commentList>
-</comments>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
@@ -68658,8 +68561,8 @@
     <dataValidation type="list" allowBlank="1" sqref="AF2:AF1999">
       <formula1>'Call Queues'!$A$2:$A$999</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" sqref="Q2:Q1999">
-      <formula1>'Flexible Fields'!$C$121:$C$130</formula1>
+    <dataValidation type="list" allowBlank="1" sqref="M2:M1999">
+      <formula1>"Never,Only when music ends,Every 15 seconds,Every 20 seconds,Every 25 seconds,Every 30 seconds,Every 40 seconds,Every 50 seconds,Every 60 seconds"</formula1>
     </dataValidation>
     <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="U2:U1999">
       <formula1>"Send new callers to voicemail,Advise callers of heavy call volume and disconnect,Send new callers to Extension →,Forward new callers to Externa number →"</formula1>
@@ -68676,38 +68579,34 @@
     <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="T2:T1999">
       <formula1>"5 Callers,10 Callers,15 Callers,20 Callers,25 Callers"</formula1>
     </dataValidation>
+    <dataValidation type="list" allowBlank="1" sqref="K2:L1999">
+      <formula1>"Ring Tones,Music (Acoustic),Music (Beautiful),Music (Classical),Music (Corporate),Music (Country),Music (Holiday),Music (Latin America),Music (Modern Jazz),Music (Nature),Music (Reggae),Music (World),None"</formula1>
+    </dataValidation>
     <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="S2:S1999">
       <formula1>"Allow,Not Allowed"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" sqref="P2:P1999">
-      <formula1>'Flexible Fields'!$C$131:$C$138</formula1>
-    </dataValidation>
-    <dataValidation type="list" allowBlank="1" sqref="N2:N1999">
-      <formula1>'Flexible Fields'!$C$115:$C$120</formula1>
+    <dataValidation type="list" allowBlank="1" sqref="Q2:Q1999">
+      <formula1>"Don't Wait,15 secs,30 secs,1 min,2 min,3 min,4 min,5 min,10 min,15 min"</formula1>
     </dataValidation>
     <dataValidation type="list" allowBlank="1" sqref="Y2:Y1999">
       <formula1>"Default,Custom"</formula1>
     </dataValidation>
     <dataValidation type="list" allowBlank="1" sqref="R2:R1999">
-      <formula1>'Flexible Fields'!$C$139:$C$147</formula1>
-    </dataValidation>
-    <dataValidation type="list" allowBlank="1" sqref="K2:K1999">
-      <formula1>'Flexible Fields'!$C$76:$C$89</formula1>
-    </dataValidation>
-    <dataValidation type="list" allowBlank="1" sqref="L2:L1999">
-      <formula1>'Flexible Fields'!$C$76:$C$89</formula1>
+      <formula1>"0 secs,10 secs,15 secs,20 secs,30 secs,45 secs,1 min,3 min,5 min"</formula1>
     </dataValidation>
     <dataValidation type="list" allowBlank="1" sqref="AC2:AC1999">
       <formula1>"Play an Announcement,Send to Voicemail,Forward to External Number →,Forward to Extension →"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" sqref="M2:M1999">
-      <formula1>'Flexible Fields'!$C$106:$C$114</formula1>
+    <dataValidation type="list" allowBlank="1" sqref="N2:N1999">
+      <formula1>"Thank you, Stay on the line,Appreciate Patience, Stay on the line,Thank you, Wait for Agent,Appreciate Patience, Wait for Agent,Custom,N/A"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" sqref="P2:P1999">
+      <formula1>"10 secs,15 secs,30 secs,45 secs,1 min,2 min,5 min,N/A (simultaneous)"</formula1>
     </dataValidation>
     <dataValidation type="list" allowBlank="1" sqref="J2:J1999">
       <formula1>"Default,Custom,Off"</formula1>
     </dataValidation>
   </dataValidations>
-  <drawing r:id="rId2"/>
-  <legacyDrawing r:id="rId3"/>
+  <drawing r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>